<commit_message>
Actualización piso I demografía
</commit_message>
<xml_diff>
--- a/Data/Indicadores demográficos proyecciones.xlsx
+++ b/Data/Indicadores demográficos proyecciones.xlsx
@@ -1,26 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Dropbox\1. Unidad de Métodos y Acceso a Datos\1. Observatorio UMAD\PISO III_INDICADORES\2021\Piso_1_Demografia\Piso-I_Demografia\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shari\Dropbox\UMAD\Sociodemografico\Piso-I_Demograf-a\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E60B8F-2EA8-46B5-B9C5-75C421A9543E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100" tabRatio="822"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="822" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicadores" sheetId="17" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -176,15 +185,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="#\ ###\ ##0"/>
-    <numFmt numFmtId="170" formatCode="#,##0.0"/>
-    <numFmt numFmtId="171" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="172" formatCode="#\ ##0"/>
-    <numFmt numFmtId="173" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="#\ ###\ ##0"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="168" formatCode="#\ ##0"/>
+    <numFmt numFmtId="169" formatCode="#,##0.000000"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -749,14 +758,14 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="22" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -769,7 +778,7 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="22" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="22" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="22" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -778,41 +787,41 @@
     <xf numFmtId="0" fontId="22" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="22" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="22" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="22" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="22" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="22" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="2" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="2" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="2"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="2" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="2" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="2" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="2" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="2" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -825,8 +834,8 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="21" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="21" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="21" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -835,79 +844,19 @@
     <xf numFmtId="0" fontId="21" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="21" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="21" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="21" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="21" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="21" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="25" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="19" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="25" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="19" fillId="25" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -915,15 +864,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -938,22 +878,22 @@
     <xf numFmtId="49" fontId="19" fillId="25" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="19" fillId="25" borderId="1" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="19" fillId="25" borderId="1" xfId="46" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="19" fillId="25" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="19" fillId="25" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="19" fillId="25" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="19" fillId="25" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="19" fillId="25" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="19" fillId="25" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="25" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="25" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -962,7 +902,7 @@
     <xf numFmtId="0" fontId="19" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="19" fillId="25" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="19" fillId="25" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -981,7 +921,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="19" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -990,9 +930,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="20" fillId="25" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="20" fillId="25" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="19" fillId="25" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="20" fillId="25" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="20" fillId="25" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="19" fillId="25" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1007,7 +947,7 @@
     <xf numFmtId="3" fontId="19" fillId="25" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="19" fillId="25" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="19" fillId="25" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="19" fillId="25" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1029,61 +969,130 @@
     <xf numFmtId="3" fontId="19" fillId="25" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="25" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="25" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="19" fillId="25" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="25" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="25" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="47">
-    <cellStyle name="20% - Accent1 2" xfId="8"/>
-    <cellStyle name="20% - Accent2 2" xfId="9"/>
-    <cellStyle name="20% - Accent3 2" xfId="10"/>
-    <cellStyle name="20% - Accent4 2" xfId="11"/>
-    <cellStyle name="20% - Accent5 2" xfId="12"/>
-    <cellStyle name="20% - Accent6 2" xfId="13"/>
-    <cellStyle name="40% - Accent1 2" xfId="14"/>
-    <cellStyle name="40% - Accent2 2" xfId="15"/>
-    <cellStyle name="40% - Accent3 2" xfId="16"/>
-    <cellStyle name="40% - Accent4 2" xfId="17"/>
-    <cellStyle name="40% - Accent5 2" xfId="18"/>
-    <cellStyle name="40% - Accent6 2" xfId="19"/>
-    <cellStyle name="60% - Accent1 2" xfId="20"/>
-    <cellStyle name="60% - Accent2 2" xfId="21"/>
-    <cellStyle name="60% - Accent3 2" xfId="22"/>
-    <cellStyle name="60% - Accent4 2" xfId="23"/>
-    <cellStyle name="60% - Accent5 2" xfId="24"/>
-    <cellStyle name="60% - Accent6 2" xfId="25"/>
-    <cellStyle name="Accent1 2" xfId="26"/>
-    <cellStyle name="Accent2 2" xfId="27"/>
-    <cellStyle name="Accent3 2" xfId="28"/>
-    <cellStyle name="Accent4 2" xfId="29"/>
-    <cellStyle name="Accent5 2" xfId="30"/>
-    <cellStyle name="Accent6 2" xfId="31"/>
-    <cellStyle name="Bad 2" xfId="32"/>
-    <cellStyle name="Calculation 2" xfId="33"/>
-    <cellStyle name="Comma 2" xfId="46"/>
-    <cellStyle name="Explanatory Text 2" xfId="34"/>
-    <cellStyle name="Heading 1 2" xfId="35"/>
-    <cellStyle name="Heading 2 2" xfId="36"/>
-    <cellStyle name="Heading 3 2" xfId="37"/>
-    <cellStyle name="Hyperlink 2" xfId="38"/>
-    <cellStyle name="Millares 2" xfId="6"/>
-    <cellStyle name="Millares 2 2" xfId="39"/>
-    <cellStyle name="Neutral 2" xfId="40"/>
+    <cellStyle name="20% - Accent1 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="20% - Accent2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20% - Accent3 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="20% - Accent4 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="20% - Accent5 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="20% - Accent6 2" xfId="13" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="40% - Accent1 2" xfId="14" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="40% - Accent2 2" xfId="15" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="40% - Accent3 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="40% - Accent4 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="40% - Accent5 2" xfId="18" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="40% - Accent6 2" xfId="19" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="60% - Accent1 2" xfId="20" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="60% - Accent2 2" xfId="21" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="60% - Accent3 2" xfId="22" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="60% - Accent4 2" xfId="23" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="60% - Accent5 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="60% - Accent6 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Accent1 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Accent2 2" xfId="27" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Accent3 2" xfId="28" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Accent4 2" xfId="29" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Accent5 2" xfId="30" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Accent6 2" xfId="31" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Bad 2" xfId="32" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Calculation 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Comma 2" xfId="46" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Explanatory Text 2" xfId="34" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Heading 1 2" xfId="35" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Heading 2 2" xfId="36" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Heading 3 2" xfId="37" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Hyperlink 2" xfId="38" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Millares 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Millares 2 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Neutral 2" xfId="40" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 2 2" xfId="5"/>
-    <cellStyle name="Normal 2 3" xfId="4"/>
-    <cellStyle name="Normal 2 4" xfId="41"/>
-    <cellStyle name="Normal 3" xfId="2"/>
-    <cellStyle name="Normal 3 2" xfId="42"/>
-    <cellStyle name="Normal 4" xfId="3"/>
-    <cellStyle name="Normal 5" xfId="7"/>
-    <cellStyle name="Output 2" xfId="43"/>
-    <cellStyle name="Title 2" xfId="44"/>
-    <cellStyle name="Total 2" xfId="45"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Normal 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Normal 2 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Normal 2 4" xfId="41" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Normal 3 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Normal 4" xfId="3" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Normal 5" xfId="7" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Output 2" xfId="43" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Title 2" xfId="44" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Total 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1110,996 +1119,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="PIRAMIDES censos ed quinquenal"/>
-      <sheetName val="PIRAMIDES censos ed simples"/>
-      <sheetName val="piran proyecciones"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="34">
-          <cell r="B34" t="str">
-            <v>Hombres</v>
-          </cell>
-          <cell r="C34" t="str">
-            <v>Mujeres</v>
-          </cell>
-          <cell r="E34" t="str">
-            <v>Hombres</v>
-          </cell>
-          <cell r="F34" t="str">
-            <v>Mujeres</v>
-          </cell>
-          <cell r="H34" t="str">
-            <v>Hombres</v>
-          </cell>
-          <cell r="I34" t="str">
-            <v>Mujeres</v>
-          </cell>
-          <cell r="K34" t="str">
-            <v>Hombres</v>
-          </cell>
-          <cell r="L34" t="str">
-            <v>Mujeres</v>
-          </cell>
-          <cell r="N34" t="str">
-            <v>Hombres</v>
-          </cell>
-          <cell r="O34" t="str">
-            <v>Mujeres</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35" t="str">
-            <v>0-4</v>
-          </cell>
-          <cell r="B35">
-            <v>-5.0372900756532468</v>
-          </cell>
-          <cell r="C35">
-            <v>4.8654003618976374</v>
-          </cell>
-          <cell r="D35" t="str">
-            <v>0-4</v>
-          </cell>
-          <cell r="E35">
-            <v>-4.6998865669522161</v>
-          </cell>
-          <cell r="F35">
-            <v>4.5276749022478251</v>
-          </cell>
-          <cell r="G35" t="str">
-            <v>0-4</v>
-          </cell>
-          <cell r="H35">
-            <v>-4.4340114939183488</v>
-          </cell>
-          <cell r="I35">
-            <v>4.261859913893753</v>
-          </cell>
-          <cell r="J35" t="str">
-            <v>0-4</v>
-          </cell>
-          <cell r="K35">
-            <v>-4.298488856466177</v>
-          </cell>
-          <cell r="L35">
-            <v>4.178473545584799</v>
-          </cell>
-          <cell r="M35" t="str">
-            <v>0-4</v>
-          </cell>
-          <cell r="N35">
-            <v>-3.430493723971634</v>
-          </cell>
-          <cell r="O35">
-            <v>3.2763857089547015</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="A36" t="str">
-            <v>5-9</v>
-          </cell>
-          <cell r="B36">
-            <v>-4.8713490445949024</v>
-          </cell>
-          <cell r="C36">
-            <v>4.7473598346499495</v>
-          </cell>
-          <cell r="D36" t="str">
-            <v>5-9</v>
-          </cell>
-          <cell r="E36">
-            <v>-4.3974223478525003</v>
-          </cell>
-          <cell r="F36">
-            <v>4.2787175144140299</v>
-          </cell>
-          <cell r="G36" t="str">
-            <v>5-9</v>
-          </cell>
-          <cell r="H36">
-            <v>-4.7418673860912897</v>
-          </cell>
-          <cell r="I36">
-            <v>4.5822371515766402</v>
-          </cell>
-          <cell r="J36" t="str">
-            <v>5-9</v>
-          </cell>
-          <cell r="K36">
-            <v>-4.2709899572123451</v>
-          </cell>
-          <cell r="L36">
-            <v>4.1330845578508884</v>
-          </cell>
-          <cell r="M36" t="str">
-            <v>5-9</v>
-          </cell>
-          <cell r="N36">
-            <v>-3.7079672900183178</v>
-          </cell>
-          <cell r="O36">
-            <v>3.5383662906751714</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="A37" t="str">
-            <v>10-14</v>
-          </cell>
-          <cell r="B37">
-            <v>-4.3883782180234974</v>
-          </cell>
-          <cell r="C37">
-            <v>4.2665663037063011</v>
-          </cell>
-          <cell r="D37" t="str">
-            <v>10-14</v>
-          </cell>
-          <cell r="E37">
-            <v>-4.6101944858556561</v>
-          </cell>
-          <cell r="F37">
-            <v>4.4757818829168681</v>
-          </cell>
-          <cell r="G37" t="str">
-            <v>10-14</v>
-          </cell>
-          <cell r="H37">
-            <v>-4.4482925960945581</v>
-          </cell>
-          <cell r="I37">
-            <v>4.2633150972908549</v>
-          </cell>
-          <cell r="J37" t="str">
-            <v>10-14</v>
-          </cell>
-          <cell r="K37">
-            <v>-4.1560635230894354</v>
-          </cell>
-          <cell r="L37">
-            <v>4.0555186971969768</v>
-          </cell>
-          <cell r="M37" t="str">
-            <v>10-14</v>
-          </cell>
-          <cell r="N37">
-            <v>-3.9880585312163848</v>
-          </cell>
-          <cell r="O37">
-            <v>3.8208925785256889</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="A38" t="str">
-            <v>15-19</v>
-          </cell>
-          <cell r="B38">
-            <v>-4.0036578566546321</v>
-          </cell>
-          <cell r="C38">
-            <v>3.9947153924692009</v>
-          </cell>
-          <cell r="D38" t="str">
-            <v>15-19</v>
-          </cell>
-          <cell r="E38">
-            <v>-4.2348218297830069</v>
-          </cell>
-          <cell r="F38">
-            <v>4.2336383676973668</v>
-          </cell>
-          <cell r="G38" t="str">
-            <v>15-19</v>
-          </cell>
-          <cell r="H38">
-            <v>-3.9197226082030379</v>
-          </cell>
-          <cell r="I38">
-            <v>3.8475725848862621</v>
-          </cell>
-          <cell r="J38" t="str">
-            <v>15-19</v>
-          </cell>
-          <cell r="K38">
-            <v>-4.2016737663345829</v>
-          </cell>
-          <cell r="L38">
-            <v>4.0627569132074681</v>
-          </cell>
-          <cell r="M38" t="str">
-            <v>15-19</v>
-          </cell>
-          <cell r="N38">
-            <v>-4.0495434591907484</v>
-          </cell>
-          <cell r="O38">
-            <v>3.9158289598880853</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="A39" t="str">
-            <v>20-24</v>
-          </cell>
-          <cell r="B39">
-            <v>-3.7024912150009448</v>
-          </cell>
-          <cell r="C39">
-            <v>3.7805628153676634</v>
-          </cell>
-          <cell r="D39" t="str">
-            <v>20-24</v>
-          </cell>
-          <cell r="E39">
-            <v>-3.5905881053453395</v>
-          </cell>
-          <cell r="F39">
-            <v>3.7174695859209614</v>
-          </cell>
-          <cell r="G39" t="str">
-            <v>20-24</v>
-          </cell>
-          <cell r="H39">
-            <v>-3.8141710497016197</v>
-          </cell>
-          <cell r="I39">
-            <v>3.865068627125837</v>
-          </cell>
-          <cell r="J39" t="str">
-            <v>20-24</v>
-          </cell>
-          <cell r="K39">
-            <v>-3.8898931430704513</v>
-          </cell>
-          <cell r="L39">
-            <v>3.8378980979295858</v>
-          </cell>
-          <cell r="M39" t="str">
-            <v>20-24</v>
-          </cell>
-          <cell r="N39">
-            <v>-3.6503784366878738</v>
-          </cell>
-          <cell r="O39">
-            <v>3.6853822323168433</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="A40" t="str">
-            <v>25-29</v>
-          </cell>
-          <cell r="B40">
-            <v>-3.5582842599411042</v>
-          </cell>
-          <cell r="C40">
-            <v>3.7134554536978643</v>
-          </cell>
-          <cell r="D40" t="str">
-            <v>25-29</v>
-          </cell>
-          <cell r="E40">
-            <v>-3.326102260448446</v>
-          </cell>
-          <cell r="F40">
-            <v>3.4468153931837606</v>
-          </cell>
-          <cell r="G40" t="str">
-            <v>25-29</v>
-          </cell>
-          <cell r="H40">
-            <v>-3.5720691421930764</v>
-          </cell>
-          <cell r="I40">
-            <v>3.7084502838284452</v>
-          </cell>
-          <cell r="J40" t="str">
-            <v>25-29</v>
-          </cell>
-          <cell r="K40">
-            <v>-3.4063550272254908</v>
-          </cell>
-          <cell r="L40">
-            <v>3.4598356450846666</v>
-          </cell>
-          <cell r="M40" t="str">
-            <v>25-29</v>
-          </cell>
-          <cell r="N40">
-            <v>-3.4349985602786668</v>
-          </cell>
-          <cell r="O40">
-            <v>3.5166030612188992</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="A41" t="str">
-            <v>30-34</v>
-          </cell>
-          <cell r="B41">
-            <v>-3.8727479570357364</v>
-          </cell>
-          <cell r="C41">
-            <v>3.9410217270775481</v>
-          </cell>
-          <cell r="D41" t="str">
-            <v>30-34</v>
-          </cell>
-          <cell r="E41">
-            <v>-3.1563651073776668</v>
-          </cell>
-          <cell r="F41">
-            <v>3.23802399128685</v>
-          </cell>
-          <cell r="G41" t="str">
-            <v>30-34</v>
-          </cell>
-          <cell r="H41">
-            <v>-3.2061074385591111</v>
-          </cell>
-          <cell r="I41">
-            <v>3.3518965100641163</v>
-          </cell>
-          <cell r="J41" t="str">
-            <v>30-34</v>
-          </cell>
-          <cell r="K41">
-            <v>-3.3805945641313841</v>
-          </cell>
-          <cell r="L41">
-            <v>3.4897367470319365</v>
-          </cell>
-          <cell r="M41" t="str">
-            <v>30-34</v>
-          </cell>
-          <cell r="N41">
-            <v>-3.4664106620952726</v>
-          </cell>
-          <cell r="O41">
-            <v>3.6367726135173091</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="A42" t="str">
-            <v>35-39</v>
-          </cell>
-          <cell r="B42">
-            <v>-3.6258193046806411</v>
-          </cell>
-          <cell r="C42">
-            <v>3.7029188980706826</v>
-          </cell>
-          <cell r="D42" t="str">
-            <v>35-39</v>
-          </cell>
-          <cell r="E42">
-            <v>-3.0714427371111115</v>
-          </cell>
-          <cell r="F42">
-            <v>3.2397812531715888</v>
-          </cell>
-          <cell r="G42" t="str">
-            <v>35-39</v>
-          </cell>
-          <cell r="H42">
-            <v>-2.9481000381055003</v>
-          </cell>
-          <cell r="I42">
-            <v>3.1208269231940666</v>
-          </cell>
-          <cell r="J42" t="str">
-            <v>35-39</v>
-          </cell>
-          <cell r="K42">
-            <v>-3.2569127333494956</v>
-          </cell>
-          <cell r="L42">
-            <v>3.4129610846324456</v>
-          </cell>
-          <cell r="M42" t="str">
-            <v>35-39</v>
-          </cell>
-          <cell r="N42">
-            <v>-3.3087413913491317</v>
-          </cell>
-          <cell r="O42">
-            <v>3.4643713105238456</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="A43" t="str">
-            <v>40-44</v>
-          </cell>
-          <cell r="B43">
-            <v>-3.2872887148434797</v>
-          </cell>
-          <cell r="C43">
-            <v>3.2091004736395594</v>
-          </cell>
-          <cell r="D43" t="str">
-            <v>40-44</v>
-          </cell>
-          <cell r="E43">
-            <v>-3.2370915666133153</v>
-          </cell>
-          <cell r="F43">
-            <v>3.3141959146171556</v>
-          </cell>
-          <cell r="G43" t="str">
-            <v>40-44</v>
-          </cell>
-          <cell r="H43">
-            <v>-2.7846118755148135</v>
-          </cell>
-          <cell r="I43">
-            <v>2.8987253270270874</v>
-          </cell>
-          <cell r="J43" t="str">
-            <v>40-44</v>
-          </cell>
-          <cell r="K43">
-            <v>-2.9492095330781729</v>
-          </cell>
-          <cell r="L43">
-            <v>3.1080077742865062</v>
-          </cell>
-          <cell r="M43" t="str">
-            <v>40-44</v>
-          </cell>
-          <cell r="N43">
-            <v>-3.0015602561425574</v>
-          </cell>
-          <cell r="O43">
-            <v>3.1803535565987024</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="A44" t="str">
-            <v>45-49</v>
-          </cell>
-          <cell r="B44">
-            <v>-2.8444034559902458</v>
-          </cell>
-          <cell r="C44">
-            <v>2.8692479543141167</v>
-          </cell>
-          <cell r="D44" t="str">
-            <v>45-49</v>
-          </cell>
-          <cell r="E44">
-            <v>-3.1640396796906072</v>
-          </cell>
-          <cell r="F44">
-            <v>3.2412516151567781</v>
-          </cell>
-          <cell r="G44" t="str">
-            <v>45-49</v>
-          </cell>
-          <cell r="H44">
-            <v>-2.6400749385608031</v>
-          </cell>
-          <cell r="I44">
-            <v>2.7981484652552968</v>
-          </cell>
-          <cell r="J44" t="str">
-            <v>45-49</v>
-          </cell>
-          <cell r="K44">
-            <v>-2.6391989539039429</v>
-          </cell>
-          <cell r="L44">
-            <v>2.7986293537158127</v>
-          </cell>
-          <cell r="M44" t="str">
-            <v>45-49</v>
-          </cell>
-          <cell r="N44">
-            <v>-2.9163336233068056</v>
-          </cell>
-          <cell r="O44">
-            <v>3.1339354797863734</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="A45" t="str">
-            <v>50-54</v>
-          </cell>
-          <cell r="B45">
-            <v>-2.7991856914352189</v>
-          </cell>
-          <cell r="C45">
-            <v>2.7191700771151455</v>
-          </cell>
-          <cell r="D45" t="str">
-            <v>50-54</v>
-          </cell>
-          <cell r="E45">
-            <v>-2.8291199094543917</v>
-          </cell>
-          <cell r="F45">
-            <v>2.8801880915741442</v>
-          </cell>
-          <cell r="G45" t="str">
-            <v>50-54</v>
-          </cell>
-          <cell r="H45">
-            <v>-2.7200761839270595</v>
-          </cell>
-          <cell r="I45">
-            <v>2.8657298895346592</v>
-          </cell>
-          <cell r="J45" t="str">
-            <v>50-54</v>
-          </cell>
-          <cell r="K45">
-            <v>-2.4140872751846456</v>
-          </cell>
-          <cell r="L45">
-            <v>2.5811351861691283</v>
-          </cell>
-          <cell r="M45" t="str">
-            <v>50-54</v>
-          </cell>
-          <cell r="N45">
-            <v>-2.8360683980254207</v>
-          </cell>
-          <cell r="O45">
-            <v>3.0861172511488855</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="A46" t="str">
-            <v>55-59</v>
-          </cell>
-          <cell r="B46">
-            <v>-2.3441309052339854</v>
-          </cell>
-          <cell r="C46">
-            <v>2.2435087430083538</v>
-          </cell>
-          <cell r="D46" t="str">
-            <v>55-59</v>
-          </cell>
-          <cell r="E46">
-            <v>-2.3337155079078578</v>
-          </cell>
-          <cell r="F46">
-            <v>2.4238738013411854</v>
-          </cell>
-          <cell r="G46" t="str">
-            <v>55-59</v>
-          </cell>
-          <cell r="H46">
-            <v>-2.5910724837002537</v>
-          </cell>
-          <cell r="I46">
-            <v>2.825153961787561</v>
-          </cell>
-          <cell r="J46" t="str">
-            <v>55-59</v>
-          </cell>
-          <cell r="K46">
-            <v>-2.2096471828009872</v>
-          </cell>
-          <cell r="L46">
-            <v>2.4581803377813065</v>
-          </cell>
-          <cell r="M46" t="str">
-            <v>55-59</v>
-          </cell>
-          <cell r="N46">
-            <v>-2.4906874684585363</v>
-          </cell>
-          <cell r="O46">
-            <v>2.7753139840467917</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="A47" t="str">
-            <v>60-64</v>
-          </cell>
-          <cell r="B47">
-            <v>-1.9849937674912654</v>
-          </cell>
-          <cell r="C47">
-            <v>1.9964245695369902</v>
-          </cell>
-          <cell r="D47" t="str">
-            <v>60-64</v>
-          </cell>
-          <cell r="E47">
-            <v>-2.1611093558415866</v>
-          </cell>
-          <cell r="F47">
-            <v>2.3868278518118986</v>
-          </cell>
-          <cell r="G47" t="str">
-            <v>60-64</v>
-          </cell>
-          <cell r="H47">
-            <v>-2.1948565019963087</v>
-          </cell>
-          <cell r="I47">
-            <v>2.4494459135404476</v>
-          </cell>
-          <cell r="J47" t="str">
-            <v>60-64</v>
-          </cell>
-          <cell r="K47">
-            <v>-2.1142544495273508</v>
-          </cell>
-          <cell r="L47">
-            <v>2.4401638175805203</v>
-          </cell>
-          <cell r="M47" t="str">
-            <v>60-64</v>
-          </cell>
-          <cell r="N47">
-            <v>-2.1265262415846311</v>
-          </cell>
-          <cell r="O47">
-            <v>2.4627757462048274</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="A48" t="str">
-            <v>65-69</v>
-          </cell>
-          <cell r="B48">
-            <v>-1.3938580045552136</v>
-          </cell>
-          <cell r="C48">
-            <v>1.5074272997101863</v>
-          </cell>
-          <cell r="D48" t="str">
-            <v>65-69</v>
-          </cell>
-          <cell r="E48">
-            <v>-1.6821658360316867</v>
-          </cell>
-          <cell r="F48">
-            <v>1.8672879962157902</v>
-          </cell>
-          <cell r="G48" t="str">
-            <v>65-69</v>
-          </cell>
-          <cell r="H48">
-            <v>-1.6836133489726066</v>
-          </cell>
-          <cell r="I48">
-            <v>2.0237878491509513</v>
-          </cell>
-          <cell r="J48" t="str">
-            <v>65-69</v>
-          </cell>
-          <cell r="K48">
-            <v>-1.9239114940025532</v>
-          </cell>
-          <cell r="L48">
-            <v>2.3634197631112066</v>
-          </cell>
-          <cell r="M48" t="str">
-            <v>65-69</v>
-          </cell>
-          <cell r="N48">
-            <v>-1.7888157089729644</v>
-          </cell>
-          <cell r="O48">
-            <v>2.215709825230614</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="A49" t="str">
-            <v>70-74</v>
-          </cell>
-          <cell r="B49">
-            <v>-0.98658708132743489</v>
-          </cell>
-          <cell r="C49">
-            <v>1.1260506423410905</v>
-          </cell>
-          <cell r="D49" t="str">
-            <v>70-74</v>
-          </cell>
-          <cell r="E49">
-            <v>-1.2357854548206175</v>
-          </cell>
-          <cell r="F49">
-            <v>1.494820201626077</v>
-          </cell>
-          <cell r="G49" t="str">
-            <v>70-74</v>
-          </cell>
-          <cell r="H49">
-            <v>-1.3412729944357848</v>
-          </cell>
-          <cell r="I49">
-            <v>1.7680478274788711</v>
-          </cell>
-          <cell r="J49" t="str">
-            <v>70-74</v>
-          </cell>
-          <cell r="K49">
-            <v>-1.4392038847410504</v>
-          </cell>
-          <cell r="L49">
-            <v>1.9036508107592129</v>
-          </cell>
-          <cell r="M49" t="str">
-            <v>70-74</v>
-          </cell>
-          <cell r="N49">
-            <v>-1.4520487569391221</v>
-          </cell>
-          <cell r="O49">
-            <v>1.9690395993374239</v>
-          </cell>
-        </row>
-        <row r="50">
-          <cell r="A50" t="str">
-            <v>75-79</v>
-          </cell>
-          <cell r="B50">
-            <v>-0.60416065642352756</v>
-          </cell>
-          <cell r="C50">
-            <v>0.77947183473704096</v>
-          </cell>
-          <cell r="D50" t="str">
-            <v>75-79</v>
-          </cell>
-          <cell r="E50">
-            <v>-0.76559238194696722</v>
-          </cell>
-          <cell r="F50">
-            <v>1.0604896161960731</v>
-          </cell>
-          <cell r="G50" t="str">
-            <v>75-79</v>
-          </cell>
-          <cell r="H50">
-            <v>-0.89172284915433542</v>
-          </cell>
-          <cell r="I50">
-            <v>1.2740638263742854</v>
-          </cell>
-          <cell r="J50" t="str">
-            <v>75-79</v>
-          </cell>
-          <cell r="K50">
-            <v>-0.94659429293534314</v>
-          </cell>
-          <cell r="L50">
-            <v>1.4341782238429364</v>
-          </cell>
-          <cell r="M50" t="str">
-            <v>75-79</v>
-          </cell>
-          <cell r="N50">
-            <v>-1.1203040886259579</v>
-          </cell>
-          <cell r="O50">
-            <v>1.7304963416467856</v>
-          </cell>
-        </row>
-        <row r="51">
-          <cell r="A51" t="str">
-            <v>80-84</v>
-          </cell>
-          <cell r="B51">
-            <v>-0.29521795895642222</v>
-          </cell>
-          <cell r="C51">
-            <v>0.44984482880624321</v>
-          </cell>
-          <cell r="D51" t="str">
-            <v>80-84</v>
-          </cell>
-          <cell r="E51">
-            <v>-0.38466104032055326</v>
-          </cell>
-          <cell r="F51">
-            <v>0.60528706307386704</v>
-          </cell>
-          <cell r="G51" t="str">
-            <v>80-84</v>
-          </cell>
-          <cell r="H51">
-            <v>-0.49005839007984558</v>
-          </cell>
-          <cell r="I51">
-            <v>0.80617160199448112</v>
-          </cell>
-          <cell r="J51" t="str">
-            <v>80-84</v>
-          </cell>
-          <cell r="K51">
-            <v>-0.5605666416858659</v>
-          </cell>
-          <cell r="L51">
-            <v>1.0252664311454429</v>
-          </cell>
-          <cell r="M51" t="str">
-            <v>80-84</v>
-          </cell>
-          <cell r="N51">
-            <v>-0.75827352757294642</v>
-          </cell>
-          <cell r="O51">
-            <v>1.3877635253144407</v>
-          </cell>
-        </row>
-        <row r="52">
-          <cell r="A52" t="str">
-            <v>85-89</v>
-          </cell>
-          <cell r="B52">
-            <v>-0.12025670315451256</v>
-          </cell>
-          <cell r="C52">
-            <v>0.2207233442638758</v>
-          </cell>
-          <cell r="D52" t="str">
-            <v>85-89</v>
-          </cell>
-          <cell r="E52">
-            <v>-0.16891231585957542</v>
-          </cell>
-          <cell r="F52">
-            <v>0.3203237378466513</v>
-          </cell>
-          <cell r="G52" t="str">
-            <v>85-89</v>
-          </cell>
-          <cell r="H52">
-            <v>-0.20152597976144468</v>
-          </cell>
-          <cell r="I52">
-            <v>0.41543793913543153</v>
-          </cell>
-          <cell r="J52" t="str">
-            <v>85-89</v>
-          </cell>
-          <cell r="K52">
-            <v>-0.26942599682719598</v>
-          </cell>
-          <cell r="L52">
-            <v>0.55914428482790901</v>
-          </cell>
-          <cell r="M52" t="str">
-            <v>85-89</v>
-          </cell>
-          <cell r="N52">
-            <v>-0.35110328920014194</v>
-          </cell>
-          <cell r="O52">
-            <v>0.78807241098230396</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="A53" t="str">
-            <v>90-94</v>
-          </cell>
-          <cell r="B53">
-            <v>-3.3786962509302104E-2</v>
-          </cell>
-          <cell r="C53">
-            <v>7.1034269855575316E-2</v>
-          </cell>
-          <cell r="D53" t="str">
-            <v>90-94</v>
-          </cell>
-          <cell r="E53">
-            <v>-4.7697108300049959E-2</v>
-          </cell>
-          <cell r="F53">
-            <v>0.10091703966642149</v>
-          </cell>
-          <cell r="G53" t="str">
-            <v>90-94</v>
-          </cell>
-          <cell r="H53">
-            <v>-5.9459470435072763E-2</v>
-          </cell>
-          <cell r="I53">
-            <v>0.13935919137827527</v>
-          </cell>
-          <cell r="J53" t="str">
-            <v>90-94</v>
-          </cell>
-          <cell r="K53">
-            <v>-8.151685192601342E-2</v>
-          </cell>
-          <cell r="L53">
-            <v>0.20219592934110425</v>
-          </cell>
-          <cell r="M53" t="str">
-            <v>90-94</v>
-          </cell>
-          <cell r="N53">
-            <v>-0.1106728703538549</v>
-          </cell>
-          <cell r="O53">
-            <v>0.31889979722149003</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="A54" t="str">
-            <v>95 y mas</v>
-          </cell>
-          <cell r="B54">
-            <v>-1.1275280929456399E-2</v>
-          </cell>
-          <cell r="C54">
-            <v>3.083206130020319E-2</v>
-          </cell>
-          <cell r="D54" t="str">
-            <v>95 y mas</v>
-          </cell>
-          <cell r="E54">
-            <v>-1.3807057665803936E-2</v>
-          </cell>
-          <cell r="F54">
-            <v>3.6113524855752109E-2</v>
-          </cell>
-          <cell r="G54" t="str">
-            <v>95 y mas</v>
-          </cell>
-          <cell r="H54">
-            <v>-1.3875004483995352E-2</v>
-          </cell>
-          <cell r="I54">
-            <v>3.8139341593811611E-2</v>
-          </cell>
-          <cell r="J54" t="str">
-            <v>95 y mas</v>
-          </cell>
-          <cell r="K54">
-            <v>-2.3863987283497531E-2</v>
-          </cell>
-          <cell r="L54">
-            <v>6.3310684144166296E-2</v>
-          </cell>
-          <cell r="M54" t="str">
-            <v>95 y mas</v>
-          </cell>
-          <cell r="N54">
-            <v>-2.2311114953073606E-2</v>
-          </cell>
-          <cell r="O54">
-            <v>8.5622327916774973E-2</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2364,40 +1383,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:FM51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
-      <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.08984375" style="2"/>
     <col min="2" max="4" width="12" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" style="2"/>
-    <col min="9" max="9" width="14.44140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="13.44140625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="13.109375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="14.88671875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="13.44140625" style="2" customWidth="1"/>
-    <col min="16" max="21" width="9.109375" style="2"/>
-    <col min="22" max="22" width="15.5546875" style="2" customWidth="1"/>
-    <col min="23" max="23" width="9.109375" style="2"/>
-    <col min="24" max="24" width="14.33203125" style="2" customWidth="1"/>
-    <col min="25" max="27" width="9.109375" style="2"/>
-    <col min="28" max="28" width="14.44140625" style="2" customWidth="1"/>
-    <col min="29" max="16384" width="9.109375" style="2"/>
+    <col min="5" max="5" width="13.6328125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.6328125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.08984375" style="2"/>
+    <col min="9" max="9" width="14.453125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.36328125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.6328125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="13.453125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="13.08984375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="14.90625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="13.453125" style="2" customWidth="1"/>
+    <col min="16" max="21" width="9.08984375" style="2"/>
+    <col min="22" max="22" width="15.54296875" style="2" customWidth="1"/>
+    <col min="23" max="23" width="9.08984375" style="2"/>
+    <col min="24" max="24" width="14.36328125" style="2" customWidth="1"/>
+    <col min="25" max="27" width="9.08984375" style="2"/>
+    <col min="28" max="28" width="14.453125" style="2" customWidth="1"/>
+    <col min="29" max="16384" width="9.08984375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:169" s="28" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:169" s="28" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="29"/>
       <c r="S1" s="30"/>
       <c r="T1" s="30"/>
@@ -2551,7 +1569,7 @@
       <c r="FL1" s="30"/>
       <c r="FM1" s="30"/>
     </row>
-    <row r="2" spans="1:169" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:169" x14ac:dyDescent="0.35">
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
@@ -2704,7 +1722,7 @@
       <c r="FL2" s="5"/>
       <c r="FM2" s="5"/>
     </row>
-    <row r="3" spans="1:169" s="31" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:169" s="31" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="28"/>
       <c r="S3" s="32"/>
       <c r="T3" s="32"/>
@@ -2858,7 +1876,7 @@
       <c r="FL3" s="32"/>
       <c r="FM3" s="32"/>
     </row>
-    <row r="4" spans="1:169" s="31" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:169" s="31" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="28"/>
       <c r="S4" s="32"/>
       <c r="T4" s="32"/>
@@ -3012,7 +2030,7 @@
       <c r="FL4" s="32"/>
       <c r="FM4" s="32"/>
     </row>
-    <row r="5" spans="1:169" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:169" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="33"/>
       <c r="B5" s="31"/>
       <c r="C5" s="31"/>
@@ -3025,7 +2043,7 @@
       <c r="J5" s="31"/>
       <c r="K5" s="31"/>
     </row>
-    <row r="6" spans="1:169" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:169" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>46</v>
       </c>
@@ -3175,7 +2193,7 @@
       <c r="EO6" s="3"/>
       <c r="EP6" s="3"/>
     </row>
-    <row r="7" spans="1:169" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:169" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -3323,64 +2341,64 @@
       <c r="EO7" s="15"/>
       <c r="EP7" s="15"/>
     </row>
-    <row r="8" spans="1:169" s="16" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:169" s="16" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="42"/>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="46" t="s">
+      <c r="C8" s="92"/>
+      <c r="D8" s="93"/>
+      <c r="E8" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="47"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="49" t="s">
+      <c r="F8" s="98"/>
+      <c r="G8" s="99"/>
+      <c r="H8" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="50" t="s">
+      <c r="I8" s="105" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="51"/>
-      <c r="K8" s="50" t="s">
+      <c r="J8" s="106"/>
+      <c r="K8" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="L8" s="52"/>
-      <c r="M8" s="51"/>
-      <c r="N8" s="46" t="s">
+      <c r="L8" s="107"/>
+      <c r="M8" s="106"/>
+      <c r="N8" s="97" t="s">
         <v>9</v>
       </c>
-      <c r="O8" s="48"/>
-      <c r="P8" s="46" t="s">
+      <c r="O8" s="99"/>
+      <c r="P8" s="97" t="s">
         <v>47</v>
       </c>
-      <c r="Q8" s="47"/>
-      <c r="R8" s="47"/>
-      <c r="S8" s="48"/>
-      <c r="T8" s="50" t="s">
+      <c r="Q8" s="98"/>
+      <c r="R8" s="98"/>
+      <c r="S8" s="99"/>
+      <c r="T8" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="U8" s="51"/>
-      <c r="V8" s="43" t="s">
+      <c r="U8" s="106"/>
+      <c r="V8" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="W8" s="45"/>
-      <c r="X8" s="53" t="s">
+      <c r="W8" s="93"/>
+      <c r="X8" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="Y8" s="50" t="s">
+      <c r="Y8" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="Z8" s="52"/>
-      <c r="AA8" s="51"/>
-      <c r="AB8" s="53" t="s">
+      <c r="Z8" s="107"/>
+      <c r="AA8" s="106"/>
+      <c r="AB8" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="AC8" s="43" t="s">
+      <c r="AC8" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="AD8" s="44"/>
-      <c r="AE8" s="45"/>
+      <c r="AD8" s="92"/>
+      <c r="AE8" s="93"/>
       <c r="AF8" s="15"/>
       <c r="AG8" s="15"/>
       <c r="AH8" s="15"/>
@@ -3497,50 +2515,50 @@
       <c r="EO8" s="15"/>
       <c r="EP8" s="15"/>
     </row>
-    <row r="9" spans="1:169" s="16" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="54"/>
-      <c r="B9" s="55"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="62" t="s">
+    <row r="9" spans="1:169" s="16" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="44"/>
+      <c r="B9" s="94"/>
+      <c r="C9" s="95"/>
+      <c r="D9" s="96"/>
+      <c r="E9" s="100"/>
+      <c r="F9" s="101"/>
+      <c r="G9" s="102"/>
+      <c r="H9" s="104"/>
+      <c r="I9" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="63"/>
-      <c r="K9" s="62" t="s">
+      <c r="J9" s="109"/>
+      <c r="K9" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="L9" s="64"/>
-      <c r="M9" s="63"/>
-      <c r="N9" s="58"/>
-      <c r="O9" s="60"/>
-      <c r="P9" s="58"/>
-      <c r="Q9" s="59"/>
-      <c r="R9" s="59"/>
-      <c r="S9" s="60"/>
-      <c r="T9" s="62" t="s">
+      <c r="L9" s="110"/>
+      <c r="M9" s="109"/>
+      <c r="N9" s="100"/>
+      <c r="O9" s="102"/>
+      <c r="P9" s="100"/>
+      <c r="Q9" s="101"/>
+      <c r="R9" s="101"/>
+      <c r="S9" s="102"/>
+      <c r="T9" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="U9" s="63"/>
-      <c r="V9" s="65"/>
-      <c r="W9" s="66"/>
-      <c r="X9" s="67" t="s">
+      <c r="U9" s="109"/>
+      <c r="V9" s="45"/>
+      <c r="W9" s="46"/>
+      <c r="X9" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="Y9" s="68" t="s">
+      <c r="Y9" s="111" t="s">
         <v>20</v>
       </c>
-      <c r="Z9" s="69"/>
-      <c r="AA9" s="70"/>
-      <c r="AB9" s="67" t="s">
+      <c r="Z9" s="112"/>
+      <c r="AA9" s="113"/>
+      <c r="AB9" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="AC9" s="71"/>
-      <c r="AD9" s="72"/>
-      <c r="AE9" s="73"/>
+      <c r="AC9" s="48"/>
+      <c r="AD9" s="49"/>
+      <c r="AE9" s="50"/>
       <c r="AF9" s="15"/>
       <c r="AG9" s="15"/>
       <c r="AH9" s="15"/>
@@ -3657,88 +2675,88 @@
       <c r="EO9" s="15"/>
       <c r="EP9" s="15"/>
     </row>
-    <row r="10" spans="1:169" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="74" t="s">
+    <row r="10" spans="1:169" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="75" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="76" t="s">
+      <c r="B10" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="77" t="s">
+      <c r="D10" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="78" t="s">
+      <c r="E10" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="79" t="s">
+      <c r="F10" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="53" t="s">
+      <c r="G10" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="80" t="s">
+      <c r="H10" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="81" t="s">
+      <c r="I10" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="82" t="s">
+      <c r="J10" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="K10" s="82" t="s">
+      <c r="K10" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="L10" s="82" t="s">
+      <c r="L10" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="M10" s="82" t="s">
+      <c r="M10" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="N10" s="83" t="s">
+      <c r="N10" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="O10" s="53" t="s">
+      <c r="O10" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="P10" s="84" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="85" t="s">
+      <c r="P10" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="R10" s="78" t="s">
+      <c r="R10" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="S10" s="86" t="s">
+      <c r="S10" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="T10" s="53" t="s">
+      <c r="T10" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="U10" s="84" t="s">
+      <c r="U10" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="V10" s="87" t="s">
+      <c r="V10" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="W10" s="88" t="s">
+      <c r="W10" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="X10" s="67" t="s">
+      <c r="X10" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="Y10" s="89"/>
-      <c r="Z10" s="90"/>
-      <c r="AA10" s="91"/>
-      <c r="AB10" s="67" t="s">
+      <c r="Y10" s="66"/>
+      <c r="Z10" s="67"/>
+      <c r="AA10" s="68"/>
+      <c r="AB10" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="AC10" s="92"/>
-      <c r="AD10" s="93"/>
-      <c r="AE10" s="66"/>
+      <c r="AC10" s="69"/>
+      <c r="AD10" s="70"/>
+      <c r="AE10" s="46"/>
       <c r="AF10" s="15"/>
       <c r="AG10" s="15"/>
       <c r="AH10" s="15"/>
@@ -3855,66 +2873,66 @@
       <c r="EO10" s="15"/>
       <c r="EP10" s="15"/>
     </row>
-    <row r="11" spans="1:169" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="94"/>
-      <c r="B11" s="95"/>
-      <c r="C11" s="96"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="97" t="s">
+    <row r="11" spans="1:169" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="71"/>
+      <c r="B11" s="72"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="74" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="79" t="s">
+      <c r="F11" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="98" t="s">
+      <c r="G11" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="97" t="s">
+      <c r="H11" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="99"/>
-      <c r="J11" s="100"/>
-      <c r="K11" s="101" t="s">
+      <c r="I11" s="76"/>
+      <c r="J11" s="77"/>
+      <c r="K11" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="L11" s="101" t="s">
+      <c r="L11" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="M11" s="101" t="s">
+      <c r="M11" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="N11" s="102"/>
-      <c r="O11" s="103"/>
-      <c r="P11" s="104"/>
-      <c r="Q11" s="103"/>
-      <c r="R11" s="103"/>
-      <c r="S11" s="105" t="s">
+      <c r="N11" s="79"/>
+      <c r="O11" s="80"/>
+      <c r="P11" s="81"/>
+      <c r="Q11" s="80"/>
+      <c r="R11" s="80"/>
+      <c r="S11" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="T11" s="106"/>
-      <c r="U11" s="107"/>
-      <c r="V11" s="108"/>
-      <c r="W11" s="109"/>
-      <c r="X11" s="110"/>
-      <c r="Y11" s="111" t="s">
+      <c r="T11" s="83"/>
+      <c r="U11" s="84"/>
+      <c r="V11" s="85"/>
+      <c r="W11" s="86"/>
+      <c r="X11" s="87"/>
+      <c r="Y11" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="Z11" s="112" t="s">
+      <c r="Z11" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="AA11" s="113" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="103" t="s">
+      <c r="AA11" s="90" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="AC11" s="113" t="s">
+      <c r="AC11" s="90" t="s">
         <v>43</v>
       </c>
-      <c r="AD11" s="113" t="s">
+      <c r="AD11" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="AE11" s="113" t="s">
+      <c r="AE11" s="90" t="s">
         <v>45</v>
       </c>
       <c r="AF11" s="15"/>
@@ -4033,7 +3051,7 @@
       <c r="EO11" s="15"/>
       <c r="EP11" s="15"/>
     </row>
-    <row r="12" spans="1:169" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:169" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="17">
         <v>2011</v>
       </c>
@@ -4243,7 +3261,7 @@
       <c r="EO12" s="15"/>
       <c r="EP12" s="15"/>
     </row>
-    <row r="13" spans="1:169" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:169" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="17">
         <v>2012</v>
       </c>
@@ -4453,7 +3471,7 @@
       <c r="EO13" s="15"/>
       <c r="EP13" s="15"/>
     </row>
-    <row r="14" spans="1:169" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:169" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="17">
         <v>2013</v>
       </c>
@@ -4663,7 +3681,7 @@
       <c r="EO14" s="15"/>
       <c r="EP14" s="15"/>
     </row>
-    <row r="15" spans="1:169" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:169" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="17">
         <v>2014</v>
       </c>
@@ -4873,7 +3891,7 @@
       <c r="EO15" s="15"/>
       <c r="EP15" s="15"/>
     </row>
-    <row r="16" spans="1:169" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:169" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="17">
         <v>2015</v>
       </c>
@@ -5083,7 +4101,7 @@
       <c r="EO16" s="15"/>
       <c r="EP16" s="15"/>
     </row>
-    <row r="17" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="17">
         <v>2016</v>
       </c>
@@ -5293,7 +4311,7 @@
       <c r="EO17" s="15"/>
       <c r="EP17" s="15"/>
     </row>
-    <row r="18" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="17">
         <v>2017</v>
       </c>
@@ -5503,7 +4521,7 @@
       <c r="EO18" s="15"/>
       <c r="EP18" s="15"/>
     </row>
-    <row r="19" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="17">
         <v>2018</v>
       </c>
@@ -5713,7 +4731,7 @@
       <c r="EO19" s="15"/>
       <c r="EP19" s="15"/>
     </row>
-    <row r="20" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="17">
         <v>2019</v>
       </c>
@@ -5923,7 +4941,7 @@
       <c r="EO20" s="15"/>
       <c r="EP20" s="15"/>
     </row>
-    <row r="21" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="17">
         <v>2020</v>
       </c>
@@ -6133,7 +5151,7 @@
       <c r="EO21" s="15"/>
       <c r="EP21" s="15"/>
     </row>
-    <row r="22" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="17">
         <v>2021</v>
       </c>
@@ -6343,7 +5361,7 @@
       <c r="EO22" s="15"/>
       <c r="EP22" s="15"/>
     </row>
-    <row r="23" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="17">
         <v>2022</v>
       </c>
@@ -6553,7 +5571,7 @@
       <c r="EO23" s="15"/>
       <c r="EP23" s="15"/>
     </row>
-    <row r="24" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="17">
         <v>2023</v>
       </c>
@@ -6763,7 +5781,7 @@
       <c r="EO24" s="15"/>
       <c r="EP24" s="15"/>
     </row>
-    <row r="25" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="17">
         <v>2024</v>
       </c>
@@ -6973,7 +5991,7 @@
       <c r="EO25" s="15"/>
       <c r="EP25" s="15"/>
     </row>
-    <row r="26" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="17">
         <v>2025</v>
       </c>
@@ -7183,7 +6201,7 @@
       <c r="EO26" s="15"/>
       <c r="EP26" s="15"/>
     </row>
-    <row r="27" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="17">
         <v>2026</v>
       </c>
@@ -7393,7 +6411,7 @@
       <c r="EO27" s="15"/>
       <c r="EP27" s="15"/>
     </row>
-    <row r="28" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="17">
         <v>2027</v>
       </c>
@@ -7603,7 +6621,7 @@
       <c r="EO28" s="15"/>
       <c r="EP28" s="15"/>
     </row>
-    <row r="29" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="17">
         <v>2028</v>
       </c>
@@ -7813,7 +6831,7 @@
       <c r="EO29" s="15"/>
       <c r="EP29" s="15"/>
     </row>
-    <row r="30" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="17">
         <v>2029</v>
       </c>
@@ -8023,7 +7041,7 @@
       <c r="EO30" s="15"/>
       <c r="EP30" s="15"/>
     </row>
-    <row r="31" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="17">
         <v>2030</v>
       </c>
@@ -8233,7 +7251,7 @@
       <c r="EO31" s="15"/>
       <c r="EP31" s="15"/>
     </row>
-    <row r="32" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="17">
         <v>2031</v>
       </c>
@@ -8443,7 +7461,7 @@
       <c r="EO32" s="15"/>
       <c r="EP32" s="15"/>
     </row>
-    <row r="33" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="17">
         <v>2032</v>
       </c>
@@ -8653,7 +7671,7 @@
       <c r="EO33" s="15"/>
       <c r="EP33" s="15"/>
     </row>
-    <row r="34" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="17">
         <v>2033</v>
       </c>
@@ -8863,7 +7881,7 @@
       <c r="EO34" s="15"/>
       <c r="EP34" s="15"/>
     </row>
-    <row r="35" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="17">
         <v>2034</v>
       </c>
@@ -9073,7 +8091,7 @@
       <c r="EO35" s="15"/>
       <c r="EP35" s="15"/>
     </row>
-    <row r="36" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="17">
         <v>2035</v>
       </c>
@@ -9283,7 +8301,7 @@
       <c r="EO36" s="15"/>
       <c r="EP36" s="15"/>
     </row>
-    <row r="37" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="17">
         <v>2036</v>
       </c>
@@ -9493,7 +8511,7 @@
       <c r="EO37" s="15"/>
       <c r="EP37" s="15"/>
     </row>
-    <row r="38" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="17">
         <v>2037</v>
       </c>
@@ -9703,7 +8721,7 @@
       <c r="EO38" s="15"/>
       <c r="EP38" s="15"/>
     </row>
-    <row r="39" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="17">
         <v>2038</v>
       </c>
@@ -9913,7 +8931,7 @@
       <c r="EO39" s="15"/>
       <c r="EP39" s="15"/>
     </row>
-    <row r="40" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="17">
         <v>2039</v>
       </c>
@@ -10123,7 +9141,7 @@
       <c r="EO40" s="15"/>
       <c r="EP40" s="15"/>
     </row>
-    <row r="41" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="17">
         <v>2040</v>
       </c>
@@ -10333,7 +9351,7 @@
       <c r="EO41" s="15"/>
       <c r="EP41" s="15"/>
     </row>
-    <row r="42" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="17">
         <v>2041</v>
       </c>
@@ -10543,7 +9561,7 @@
       <c r="EO42" s="15"/>
       <c r="EP42" s="15"/>
     </row>
-    <row r="43" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="17">
         <v>2042</v>
       </c>
@@ -10753,7 +9771,7 @@
       <c r="EO43" s="15"/>
       <c r="EP43" s="15"/>
     </row>
-    <row r="44" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="17">
         <v>2043</v>
       </c>
@@ -10963,7 +9981,7 @@
       <c r="EO44" s="15"/>
       <c r="EP44" s="15"/>
     </row>
-    <row r="45" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="17">
         <v>2044</v>
       </c>
@@ -11173,7 +10191,7 @@
       <c r="EO45" s="15"/>
       <c r="EP45" s="15"/>
     </row>
-    <row r="46" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="17">
         <v>2045</v>
       </c>
@@ -11383,7 +10401,7 @@
       <c r="EO46" s="15"/>
       <c r="EP46" s="15"/>
     </row>
-    <row r="47" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="17">
         <v>2046</v>
       </c>
@@ -11593,7 +10611,7 @@
       <c r="EO47" s="15"/>
       <c r="EP47" s="15"/>
     </row>
-    <row r="48" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="17">
         <v>2047</v>
       </c>
@@ -11803,7 +10821,7 @@
       <c r="EO48" s="15"/>
       <c r="EP48" s="15"/>
     </row>
-    <row r="49" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="17">
         <v>2048</v>
       </c>
@@ -12013,7 +11031,7 @@
       <c r="EO49" s="15"/>
       <c r="EP49" s="15"/>
     </row>
-    <row r="50" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="17">
         <v>2049</v>
       </c>
@@ -12223,7 +11241,7 @@
       <c r="EO50" s="15"/>
       <c r="EP50" s="15"/>
     </row>
-    <row r="51" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:146" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="17">
         <v>2050</v>
       </c>
@@ -12435,13 +11453,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B8:D9"/>
-    <mergeCell ref="E8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:M9"/>
     <mergeCell ref="AC8:AE8"/>
     <mergeCell ref="T9:U9"/>
     <mergeCell ref="Y9:AA9"/>
@@ -12450,6 +11461,13 @@
     <mergeCell ref="T8:U8"/>
     <mergeCell ref="V8:W8"/>
     <mergeCell ref="Y8:AA8"/>
+    <mergeCell ref="B8:D9"/>
+    <mergeCell ref="E8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:M8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:M9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>